<commit_message>
Add To Cart Validation Functionalities
</commit_message>
<xml_diff>
--- a/src/test/java/Org/data/RegistrationData.xlsx
+++ b/src/test/java/Org/data/RegistrationData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santa\IdeaProjects\Santanu_SwagLabs\src\test\java\Org\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D106008-980F-4DF2-A3FB-3C272BA4756D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E236CE30-0F03-4572-ACBE-F8FD57823F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C5D391E-A33B-46FC-BA6C-C9344314E494}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7C5D391E-A33B-46FC-BA6C-C9344314E494}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="AddProductTest" sheetId="3" r:id="rId2"/>
     <sheet name="InValidLoginDetails" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack;Test.allTheThings() T-Shirt (Red);Sauce Labs Bike Light</t>
   </si>
 </sst>
 </file>
@@ -473,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4A0914-D2C3-419C-918E-202D06A59A09}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,18 +520,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1220268B-159C-4630-97C8-3BCD6984DD22}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.21875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Cart Page related changes
</commit_message>
<xml_diff>
--- a/src/test/java/Org/data/RegistrationData.xlsx
+++ b/src/test/java/Org/data/RegistrationData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santa\IdeaProjects\Santanu_SwagLabs\src\test\java\Org\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E236CE30-0F03-4572-ACBE-F8FD57823F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6403AC99-069A-4430-97A5-E76F5EE595AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7C5D391E-A33B-46FC-BA6C-C9344314E494}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7C5D391E-A33B-46FC-BA6C-C9344314E494}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
     <sheet name="AddProductTest" sheetId="3" r:id="rId2"/>
-    <sheet name="InValidLoginDetails" sheetId="2" r:id="rId3"/>
+    <sheet name="CartTest" sheetId="4" r:id="rId3"/>
+    <sheet name="InValidLoginDetails" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -522,6 +523,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1220268B-159C-4630-97C8-3BCD6984DD22}">
   <dimension ref="A1:C2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96897E27-CFAE-4D52-8DC4-15A5B3D23A0B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -560,7 +603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE7FA87-F3CA-4CEB-8840-23ED62030816}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>